<commit_message>
Added some conversions in ktk.loadmat
</commit_message>
<xml_diff>
--- a/conversion_state.xlsx
+++ b/conversion_state.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Documents/Recherche/pyKTK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8447BA55-4A4E-AD40-B36B-BB92E71DF8AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F072101F-C1E6-2C42-9B9A-E2105E883FE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="38360" windowHeight="21120" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="146">
   <si>
     <t>Module</t>
   </si>
@@ -417,12 +417,6 @@
     <t>in module gui</t>
   </si>
   <si>
-    <t>hard</t>
-  </si>
-  <si>
-    <t>No btk for python3</t>
-  </si>
-  <si>
     <t>Try to use mokka before</t>
   </si>
   <si>
@@ -459,10 +453,16 @@
     <t>Using py-c3d which I just forked</t>
   </si>
   <si>
-    <t>py-c3d write doesn't seem to allow marker labels, do I have to modify py-c3d</t>
-  </si>
-  <si>
     <t>read_c3d_file</t>
+  </si>
+  <si>
+    <t>to become write_mvc_file (for the segments)</t>
+  </si>
+  <si>
+    <t>I modified py-c3d. Not yet working on Windows, just have to launch the command line correctly.</t>
+  </si>
+  <si>
+    <t>ts.events = []</t>
   </si>
 </sst>
 </file>
@@ -519,7 +519,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="39">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -564,321 +564,6 @@
       <font>
         <color rgb="FF9C0006"/>
       </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFDE88A4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1207,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF09E79-E66E-9E44-A75F-B1B1B21A0B2B}">
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1260,10 +945,10 @@
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" t="s">
-        <v>92</v>
+        <v>107</v>
+      </c>
+      <c r="F3" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1404,11 +1089,8 @@
       <c r="B17" t="s">
         <v>15</v>
       </c>
-      <c r="D17" t="s">
-        <v>90</v>
-      </c>
-      <c r="E17" t="s">
-        <v>92</v>
+      <c r="C17" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1832,10 +1514,10 @@
         <v>90</v>
       </c>
       <c r="E49" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="F49" t="s">
-        <v>131</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1877,7 +1559,7 @@
         <v>90</v>
       </c>
       <c r="E52" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="F52" t="s">
         <v>144</v>
@@ -1905,10 +1587,10 @@
         <v>62</v>
       </c>
       <c r="C54" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="F54" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1974,11 +1656,8 @@
       <c r="D59" t="s">
         <v>119</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>130</v>
-      </c>
-      <c r="F59" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1991,11 +1670,8 @@
       <c r="D60" t="s">
         <v>119</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>130</v>
-      </c>
-      <c r="F60" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2006,7 +1682,7 @@
         <v>71</v>
       </c>
       <c r="C61" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2045,7 +1721,7 @@
         <v>74</v>
       </c>
       <c r="C64" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2056,7 +1732,7 @@
         <v>75</v>
       </c>
       <c r="C65" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2103,7 +1779,7 @@
         <v>63</v>
       </c>
       <c r="C69" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2114,7 +1790,7 @@
         <v>78</v>
       </c>
       <c r="C70" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2181,7 +1857,7 @@
         <v>84</v>
       </c>
       <c r="C75" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2222,26 +1898,26 @@
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C79" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
+        <v>137</v>
+      </c>
+      <c r="C80" t="s">
         <v>139</v>
-      </c>
-      <c r="C80" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C81" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2442,30 +2118,30 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A97:XFD97">
-    <cfRule type="expression" dxfId="13" priority="8">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>($C97&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD96">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>($C2="N/A")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>AND(($C2&lt;&gt;""),($C2&lt;&gt;"N/A"))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD96">
-    <cfRule type="expression" dxfId="10" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>($E2="easy")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD96">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>($E2="moderate")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:XFD96">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>($E2="hard")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Finished first working and tested prototypes of kinematics.write_c3d_file and kinematics.open_in_mokka.
</commit_message>
<xml_diff>
--- a/conversion_state.xlsx
+++ b/conversion_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Documents/Recherche/pyKTK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F072101F-C1E6-2C42-9B9A-E2105E883FE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2258DBFE-6D86-3F4E-9A65-D65E73194794}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="146">
   <si>
     <t>Module</t>
   </si>
@@ -372,9 +372,6 @@
     <t>moderate</t>
   </si>
   <si>
-    <t>Too specialized for a method, I have to think more about there it should be implemented</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -387,9 +384,6 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>A bit too specialized for a method. TBD.</t>
-  </si>
-  <si>
     <t>savgol</t>
   </si>
   <si>
@@ -463,6 +457,12 @@
   </si>
   <si>
     <t>ts.events = []</t>
+  </si>
+  <si>
+    <t>Maybe make a ktk.cycles submodule for cycle analysis</t>
+  </si>
+  <si>
+    <t>Maybe transfer to "extract_cycles(start_event_name, stop_event_name)" that creates a dict of (n_cycles x 100 x data_dim) arrays</t>
   </si>
 </sst>
 </file>
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF09E79-E66E-9E44-A75F-B1B1B21A0B2B}">
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -917,13 +917,13 @@
         <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -942,13 +942,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F3" t="s">
-        <v>145</v>
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -956,13 +956,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>114</v>
+      </c>
+      <c r="F4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -970,27 +973,18 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F5" t="s">
-        <v>115</v>
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -998,26 +992,26 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>1</v>
       </c>
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
-        <v>102</v>
-      </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1025,26 +1019,26 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>1</v>
       </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1052,34 +1046,37 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>1</v>
       </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>1</v>
       </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1087,10 +1084,10 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1098,10 +1095,16 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1109,16 +1112,13 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
         <v>90</v>
       </c>
       <c r="E19" t="s">
         <v>92</v>
-      </c>
-      <c r="F19" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1126,7 +1126,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
         <v>90</v>
@@ -1140,7 +1140,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
         <v>90</v>
@@ -1154,13 +1154,16 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
         <v>90</v>
       </c>
       <c r="E22" t="s">
-        <v>92</v>
+        <v>114</v>
+      </c>
+      <c r="F22" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1168,16 +1171,10 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" t="s">
-        <v>119</v>
-      </c>
-      <c r="E23" t="s">
-        <v>114</v>
-      </c>
-      <c r="F23" t="s">
-        <v>120</v>
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1185,10 +1182,10 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1196,24 +1193,21 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" t="s">
-        <v>111</v>
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>1</v>
       </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" t="s">
-        <v>114</v>
+      <c r="C26" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1221,7 +1215,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1229,15 +1223,21 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>94</v>
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1245,13 +1245,13 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D30" t="s">
         <v>90</v>
       </c>
       <c r="E30" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1259,13 +1259,10 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" t="s">
-        <v>90</v>
-      </c>
-      <c r="E31" t="s">
-        <v>92</v>
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1273,21 +1270,24 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="D33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1295,7 +1295,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
         <v>90</v>
@@ -1309,7 +1309,7 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D35" t="s">
         <v>90</v>
@@ -1323,7 +1323,7 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
         <v>90</v>
@@ -1337,13 +1337,13 @@
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
         <v>90</v>
       </c>
       <c r="E37" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1351,7 +1351,7 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D38" t="s">
         <v>90</v>
@@ -1365,7 +1365,7 @@
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
         <v>90</v>
@@ -1379,13 +1379,13 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D40" t="s">
         <v>90</v>
       </c>
       <c r="E40" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1393,27 +1393,30 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D41" t="s">
         <v>90</v>
       </c>
       <c r="E41" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D42" t="s">
         <v>90</v>
       </c>
       <c r="E42" t="s">
-        <v>114</v>
+        <v>92</v>
+      </c>
+      <c r="F42" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1421,10 +1424,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D43" t="s">
-        <v>119</v>
+        <v>90</v>
+      </c>
+      <c r="E43" t="s">
+        <v>114</v>
+      </c>
+      <c r="F43" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1432,7 +1441,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D44" t="s">
         <v>90</v>
@@ -1441,24 +1450,21 @@
         <v>114</v>
       </c>
       <c r="F44" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D45" t="s">
         <v>90</v>
       </c>
       <c r="E45" t="s">
         <v>114</v>
-      </c>
-      <c r="F45" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1466,7 +1472,7 @@
         <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D46" t="s">
         <v>90</v>
@@ -1480,7 +1486,7 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D47" t="s">
         <v>90</v>
@@ -1494,13 +1500,16 @@
         <v>53</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D48" t="s">
         <v>90</v>
       </c>
       <c r="E48" t="s">
-        <v>114</v>
+        <v>92</v>
+      </c>
+      <c r="F48" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1508,16 +1517,13 @@
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D49" t="s">
         <v>90</v>
       </c>
       <c r="E49" t="s">
         <v>92</v>
-      </c>
-      <c r="F49" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1525,7 +1531,7 @@
         <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D50" t="s">
         <v>90</v>
@@ -1539,13 +1545,16 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D51" t="s">
         <v>90</v>
       </c>
       <c r="E51" t="s">
         <v>92</v>
+      </c>
+      <c r="F51" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1553,16 +1562,13 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D52" t="s">
         <v>90</v>
       </c>
       <c r="E52" t="s">
         <v>92</v>
-      </c>
-      <c r="F52" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1570,13 +1576,13 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>61</v>
-      </c>
-      <c r="D53" t="s">
-        <v>90</v>
-      </c>
-      <c r="E53" t="s">
-        <v>92</v>
+        <v>62</v>
+      </c>
+      <c r="C53" t="s">
+        <v>140</v>
+      </c>
+      <c r="F53" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1584,13 +1590,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" t="s">
-        <v>142</v>
-      </c>
-      <c r="F54" t="s">
-        <v>141</v>
+        <v>63</v>
+      </c>
+      <c r="D54" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1598,10 +1601,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D55" t="s">
-        <v>119</v>
+        <v>90</v>
+      </c>
+      <c r="E55" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1609,13 +1615,13 @@
         <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D56" t="s">
         <v>90</v>
       </c>
       <c r="E56" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1623,27 +1629,27 @@
         <v>53</v>
       </c>
       <c r="B57" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D57" t="s">
         <v>90</v>
       </c>
       <c r="E57" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B58" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D58" t="s">
-        <v>90</v>
-      </c>
-      <c r="E58" t="s">
-        <v>114</v>
+        <v>118</v>
+      </c>
+      <c r="F58" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1651,27 +1657,24 @@
         <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F59" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
-      </c>
-      <c r="D60" t="s">
-        <v>119</v>
-      </c>
-      <c r="F60" t="s">
-        <v>130</v>
+        <v>71</v>
+      </c>
+      <c r="C60" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1679,10 +1682,13 @@
         <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>71</v>
-      </c>
-      <c r="C61" t="s">
-        <v>131</v>
+        <v>72</v>
+      </c>
+      <c r="D61" t="s">
+        <v>90</v>
+      </c>
+      <c r="E61" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1690,7 +1696,7 @@
         <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D62" t="s">
         <v>90</v>
@@ -1704,13 +1710,10 @@
         <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>73</v>
-      </c>
-      <c r="D63" t="s">
-        <v>90</v>
-      </c>
-      <c r="E63" t="s">
-        <v>92</v>
+        <v>74</v>
+      </c>
+      <c r="C63" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1718,10 +1721,10 @@
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1729,10 +1732,13 @@
         <v>70</v>
       </c>
       <c r="B65" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" t="s">
-        <v>133</v>
+        <v>59</v>
+      </c>
+      <c r="D65" t="s">
+        <v>90</v>
+      </c>
+      <c r="E65" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1740,13 +1746,10 @@
         <v>70</v>
       </c>
       <c r="B66" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D66" t="s">
-        <v>90</v>
-      </c>
-      <c r="E66" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1754,10 +1757,10 @@
         <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D67" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1765,10 +1768,10 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
-      </c>
-      <c r="D68" t="s">
-        <v>119</v>
+        <v>63</v>
+      </c>
+      <c r="C68" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1776,10 +1779,10 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1787,32 +1790,35 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
-      </c>
-      <c r="C70" t="s">
-        <v>135</v>
+        <v>79</v>
+      </c>
+      <c r="D70" t="s">
+        <v>90</v>
+      </c>
+      <c r="E70" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B71" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D71" t="s">
         <v>90</v>
       </c>
       <c r="E71" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B72" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="D72" t="s">
         <v>90</v>
@@ -1826,7 +1832,7 @@
         <v>81</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D73" t="s">
         <v>90</v>
@@ -1840,13 +1846,10 @@
         <v>81</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
-      </c>
-      <c r="D74" t="s">
-        <v>90</v>
-      </c>
-      <c r="E74" t="s">
-        <v>92</v>
+        <v>84</v>
+      </c>
+      <c r="C74" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1854,10 +1857,13 @@
         <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
-      </c>
-      <c r="C75" t="s">
-        <v>136</v>
+        <v>59</v>
+      </c>
+      <c r="D75" t="s">
+        <v>90</v>
+      </c>
+      <c r="E75" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1865,13 +1871,10 @@
         <v>81</v>
       </c>
       <c r="B76" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="D76" t="s">
-        <v>90</v>
-      </c>
-      <c r="E76" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1879,45 +1882,48 @@
         <v>81</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D77" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>81</v>
-      </c>
-      <c r="B78" t="s">
-        <v>86</v>
-      </c>
-      <c r="D78" t="s">
-        <v>119</v>
+        <v>135</v>
+      </c>
+      <c r="C78" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
+        <v>135</v>
+      </c>
+      <c r="C79" t="s">
         <v>137</v>
-      </c>
-      <c r="C79" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C80" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>137</v>
+        <v>1</v>
+      </c>
+      <c r="B81" t="s">
+        <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>140</v>
+        <v>107</v>
+      </c>
+      <c r="F81" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -1925,13 +1931,13 @@
         <v>1</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C82" t="s">
         <v>107</v>
       </c>
       <c r="F82" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -1939,13 +1945,13 @@
         <v>1</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
         <v>107</v>
       </c>
       <c r="F83" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -1953,13 +1959,13 @@
         <v>1</v>
       </c>
       <c r="B84" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C84" t="s">
         <v>107</v>
       </c>
       <c r="F84" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -1967,13 +1973,13 @@
         <v>1</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C85" t="s">
         <v>107</v>
       </c>
       <c r="F85" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -1981,13 +1987,13 @@
         <v>1</v>
       </c>
       <c r="B86" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C86" t="s">
         <v>107</v>
       </c>
       <c r="F86" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -1995,13 +2001,13 @@
         <v>1</v>
       </c>
       <c r="B87" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C87" t="s">
         <v>107</v>
       </c>
       <c r="F87" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2009,13 +2015,13 @@
         <v>1</v>
       </c>
       <c r="B88" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C88" t="s">
         <v>107</v>
       </c>
       <c r="F88" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2029,7 +2035,7 @@
         <v>107</v>
       </c>
       <c r="F89" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2043,7 +2049,7 @@
         <v>107</v>
       </c>
       <c r="F90" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2071,7 +2077,7 @@
         <v>107</v>
       </c>
       <c r="F92" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2085,7 +2091,7 @@
         <v>107</v>
       </c>
       <c r="F93" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2099,7 +2105,7 @@
         <v>107</v>
       </c>
       <c r="F94" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2113,7 +2119,7 @@
         <v>107</v>
       </c>
       <c r="F95" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[STABLE] Finished first working and tested prototypes of kinematics.write_c3d_file and kinematics.open_in_mokka.
</commit_message>
<xml_diff>
--- a/conversion_state.xlsx
+++ b/conversion_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Documents/Recherche/pyKTK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F072101F-C1E6-2C42-9B9A-E2105E883FE8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2258DBFE-6D86-3F4E-9A65-D65E73194794}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="146">
   <si>
     <t>Module</t>
   </si>
@@ -372,9 +372,6 @@
     <t>moderate</t>
   </si>
   <si>
-    <t>Too specialized for a method, I have to think more about there it should be implemented</t>
-  </si>
-  <si>
     <t>Note</t>
   </si>
   <si>
@@ -387,9 +384,6 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>A bit too specialized for a method. TBD.</t>
-  </si>
-  <si>
     <t>savgol</t>
   </si>
   <si>
@@ -463,6 +457,12 @@
   </si>
   <si>
     <t>ts.events = []</t>
+  </si>
+  <si>
+    <t>Maybe make a ktk.cycles submodule for cycle analysis</t>
+  </si>
+  <si>
+    <t>Maybe transfer to "extract_cycles(start_event_name, stop_event_name)" that creates a dict of (n_cycles x 100 x data_dim) arrays</t>
   </si>
 </sst>
 </file>
@@ -892,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF09E79-E66E-9E44-A75F-B1B1B21A0B2B}">
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -917,13 +917,13 @@
         <v>87</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>91</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -942,13 +942,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
-      </c>
-      <c r="F3" t="s">
-        <v>145</v>
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -956,13 +956,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>118</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>114</v>
+      </c>
+      <c r="F4" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -970,27 +973,18 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F5" t="s">
-        <v>115</v>
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -998,26 +992,26 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>1</v>
       </c>
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
       <c r="C8" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
-        <v>102</v>
-      </c>
       <c r="C9" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1025,26 +1019,26 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>1</v>
       </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
       <c r="C11" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>1</v>
       </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
       <c r="C12" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1052,34 +1046,37 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>1</v>
       </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="B15" t="s">
-        <v>13</v>
-      </c>
       <c r="C15" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>1</v>
       </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1087,10 +1084,10 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1098,10 +1095,16 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1109,16 +1112,13 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D19" t="s">
         <v>90</v>
       </c>
       <c r="E19" t="s">
         <v>92</v>
-      </c>
-      <c r="F19" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1126,7 +1126,7 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
         <v>90</v>
@@ -1140,7 +1140,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D21" t="s">
         <v>90</v>
@@ -1154,13 +1154,16 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
         <v>90</v>
       </c>
       <c r="E22" t="s">
-        <v>92</v>
+        <v>114</v>
+      </c>
+      <c r="F22" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1168,16 +1171,10 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="D23" t="s">
-        <v>119</v>
-      </c>
-      <c r="E23" t="s">
-        <v>114</v>
-      </c>
-      <c r="F23" t="s">
-        <v>120</v>
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1185,10 +1182,10 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1196,24 +1193,21 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" t="s">
-        <v>111</v>
+        <v>26</v>
+      </c>
+      <c r="D25" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>1</v>
       </c>
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" t="s">
-        <v>114</v>
+      <c r="C26" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1221,7 +1215,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1229,15 +1223,21 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>94</v>
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1245,13 +1245,13 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D30" t="s">
         <v>90</v>
       </c>
       <c r="E30" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1259,13 +1259,10 @@
         <v>27</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D31" t="s">
-        <v>90</v>
-      </c>
-      <c r="E31" t="s">
-        <v>92</v>
+        <v>30</v>
+      </c>
+      <c r="C31" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1273,21 +1270,24 @@
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
-        <v>121</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
-      </c>
-      <c r="C33" t="s">
-        <v>31</v>
+        <v>33</v>
+      </c>
+      <c r="D33" t="s">
+        <v>90</v>
+      </c>
+      <c r="E33" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1295,7 +1295,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
         <v>90</v>
@@ -1309,7 +1309,7 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D35" t="s">
         <v>90</v>
@@ -1323,7 +1323,7 @@
         <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
         <v>90</v>
@@ -1337,13 +1337,13 @@
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D37" t="s">
         <v>90</v>
       </c>
       <c r="E37" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1351,7 +1351,7 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D38" t="s">
         <v>90</v>
@@ -1365,7 +1365,7 @@
         <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D39" t="s">
         <v>90</v>
@@ -1379,13 +1379,13 @@
         <v>32</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D40" t="s">
         <v>90</v>
       </c>
       <c r="E40" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1393,27 +1393,30 @@
         <v>32</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D41" t="s">
         <v>90</v>
       </c>
       <c r="E41" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D42" t="s">
         <v>90</v>
       </c>
       <c r="E42" t="s">
-        <v>114</v>
+        <v>92</v>
+      </c>
+      <c r="F42" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1421,10 +1424,16 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D43" t="s">
-        <v>119</v>
+        <v>90</v>
+      </c>
+      <c r="E43" t="s">
+        <v>114</v>
+      </c>
+      <c r="F43" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1432,7 +1441,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D44" t="s">
         <v>90</v>
@@ -1441,24 +1450,21 @@
         <v>114</v>
       </c>
       <c r="F44" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D45" t="s">
         <v>90</v>
       </c>
       <c r="E45" t="s">
         <v>114</v>
-      </c>
-      <c r="F45" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1466,7 +1472,7 @@
         <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D46" t="s">
         <v>90</v>
@@ -1480,7 +1486,7 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D47" t="s">
         <v>90</v>
@@ -1494,13 +1500,16 @@
         <v>53</v>
       </c>
       <c r="B48" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D48" t="s">
         <v>90</v>
       </c>
       <c r="E48" t="s">
-        <v>114</v>
+        <v>92</v>
+      </c>
+      <c r="F48" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1508,16 +1517,13 @@
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D49" t="s">
         <v>90</v>
       </c>
       <c r="E49" t="s">
         <v>92</v>
-      </c>
-      <c r="F49" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1525,7 +1531,7 @@
         <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D50" t="s">
         <v>90</v>
@@ -1539,13 +1545,16 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D51" t="s">
         <v>90</v>
       </c>
       <c r="E51" t="s">
         <v>92</v>
+      </c>
+      <c r="F51" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1553,16 +1562,13 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D52" t="s">
         <v>90</v>
       </c>
       <c r="E52" t="s">
         <v>92</v>
-      </c>
-      <c r="F52" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1570,13 +1576,13 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>61</v>
-      </c>
-      <c r="D53" t="s">
-        <v>90</v>
-      </c>
-      <c r="E53" t="s">
-        <v>92</v>
+        <v>62</v>
+      </c>
+      <c r="C53" t="s">
+        <v>140</v>
+      </c>
+      <c r="F53" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1584,13 +1590,10 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" t="s">
-        <v>142</v>
-      </c>
-      <c r="F54" t="s">
-        <v>141</v>
+        <v>63</v>
+      </c>
+      <c r="D54" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1598,10 +1601,13 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D55" t="s">
-        <v>119</v>
+        <v>90</v>
+      </c>
+      <c r="E55" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1609,13 +1615,13 @@
         <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D56" t="s">
         <v>90</v>
       </c>
       <c r="E56" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1623,27 +1629,27 @@
         <v>53</v>
       </c>
       <c r="B57" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D57" t="s">
         <v>90</v>
       </c>
       <c r="E57" t="s">
-        <v>92</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B58" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D58" t="s">
-        <v>90</v>
-      </c>
-      <c r="E58" t="s">
-        <v>114</v>
+        <v>118</v>
+      </c>
+      <c r="F58" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1651,27 +1657,24 @@
         <v>67</v>
       </c>
       <c r="B59" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D59" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F59" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
-      </c>
-      <c r="D60" t="s">
-        <v>119</v>
-      </c>
-      <c r="F60" t="s">
-        <v>130</v>
+        <v>71</v>
+      </c>
+      <c r="C60" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1679,10 +1682,13 @@
         <v>70</v>
       </c>
       <c r="B61" t="s">
-        <v>71</v>
-      </c>
-      <c r="C61" t="s">
-        <v>131</v>
+        <v>72</v>
+      </c>
+      <c r="D61" t="s">
+        <v>90</v>
+      </c>
+      <c r="E61" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1690,7 +1696,7 @@
         <v>70</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D62" t="s">
         <v>90</v>
@@ -1704,13 +1710,10 @@
         <v>70</v>
       </c>
       <c r="B63" t="s">
-        <v>73</v>
-      </c>
-      <c r="D63" t="s">
-        <v>90</v>
-      </c>
-      <c r="E63" t="s">
-        <v>92</v>
+        <v>74</v>
+      </c>
+      <c r="C63" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1718,10 +1721,10 @@
         <v>70</v>
       </c>
       <c r="B64" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1729,10 +1732,13 @@
         <v>70</v>
       </c>
       <c r="B65" t="s">
-        <v>75</v>
-      </c>
-      <c r="C65" t="s">
-        <v>133</v>
+        <v>59</v>
+      </c>
+      <c r="D65" t="s">
+        <v>90</v>
+      </c>
+      <c r="E65" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1740,13 +1746,10 @@
         <v>70</v>
       </c>
       <c r="B66" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="D66" t="s">
-        <v>90</v>
-      </c>
-      <c r="E66" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1754,10 +1757,10 @@
         <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D67" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -1765,10 +1768,10 @@
         <v>70</v>
       </c>
       <c r="B68" t="s">
-        <v>77</v>
-      </c>
-      <c r="D68" t="s">
-        <v>119</v>
+        <v>63</v>
+      </c>
+      <c r="C68" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -1776,10 +1779,10 @@
         <v>70</v>
       </c>
       <c r="B69" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="C69" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -1787,32 +1790,35 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>78</v>
-      </c>
-      <c r="C70" t="s">
-        <v>135</v>
+        <v>79</v>
+      </c>
+      <c r="D70" t="s">
+        <v>90</v>
+      </c>
+      <c r="E70" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B71" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D71" t="s">
         <v>90</v>
       </c>
       <c r="E71" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B72" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="D72" t="s">
         <v>90</v>
@@ -1826,7 +1832,7 @@
         <v>81</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D73" t="s">
         <v>90</v>
@@ -1840,13 +1846,10 @@
         <v>81</v>
       </c>
       <c r="B74" t="s">
-        <v>83</v>
-      </c>
-      <c r="D74" t="s">
-        <v>90</v>
-      </c>
-      <c r="E74" t="s">
-        <v>92</v>
+        <v>84</v>
+      </c>
+      <c r="C74" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1854,10 +1857,13 @@
         <v>81</v>
       </c>
       <c r="B75" t="s">
-        <v>84</v>
-      </c>
-      <c r="C75" t="s">
-        <v>136</v>
+        <v>59</v>
+      </c>
+      <c r="D75" t="s">
+        <v>90</v>
+      </c>
+      <c r="E75" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1865,13 +1871,10 @@
         <v>81</v>
       </c>
       <c r="B76" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="D76" t="s">
-        <v>90</v>
-      </c>
-      <c r="E76" t="s">
-        <v>92</v>
+        <v>118</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1879,45 +1882,48 @@
         <v>81</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D77" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>81</v>
-      </c>
-      <c r="B78" t="s">
-        <v>86</v>
-      </c>
-      <c r="D78" t="s">
-        <v>119</v>
+        <v>135</v>
+      </c>
+      <c r="C78" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
+        <v>135</v>
+      </c>
+      <c r="C79" t="s">
         <v>137</v>
-      </c>
-      <c r="C79" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C80" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>137</v>
+        <v>1</v>
+      </c>
+      <c r="B81" t="s">
+        <v>4</v>
       </c>
       <c r="C81" t="s">
-        <v>140</v>
+        <v>107</v>
+      </c>
+      <c r="F81" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -1925,13 +1931,13 @@
         <v>1</v>
       </c>
       <c r="B82" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C82" t="s">
         <v>107</v>
       </c>
       <c r="F82" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -1939,13 +1945,13 @@
         <v>1</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C83" t="s">
         <v>107</v>
       </c>
       <c r="F83" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -1953,13 +1959,13 @@
         <v>1</v>
       </c>
       <c r="B84" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C84" t="s">
         <v>107</v>
       </c>
       <c r="F84" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -1967,13 +1973,13 @@
         <v>1</v>
       </c>
       <c r="B85" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C85" t="s">
         <v>107</v>
       </c>
       <c r="F85" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -1981,13 +1987,13 @@
         <v>1</v>
       </c>
       <c r="B86" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="C86" t="s">
         <v>107</v>
       </c>
       <c r="F86" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -1995,13 +2001,13 @@
         <v>1</v>
       </c>
       <c r="B87" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C87" t="s">
         <v>107</v>
       </c>
       <c r="F87" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2009,13 +2015,13 @@
         <v>1</v>
       </c>
       <c r="B88" t="s">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="C88" t="s">
         <v>107</v>
       </c>
       <c r="F88" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2029,7 +2035,7 @@
         <v>107</v>
       </c>
       <c r="F89" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2043,7 +2049,7 @@
         <v>107</v>
       </c>
       <c r="F90" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2071,7 +2077,7 @@
         <v>107</v>
       </c>
       <c r="F92" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2085,7 +2091,7 @@
         <v>107</v>
       </c>
       <c r="F93" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2099,7 +2105,7 @@
         <v>107</v>
       </c>
       <c r="F94" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2113,7 +2119,7 @@
         <v>107</v>
       </c>
       <c r="F95" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[STABLE] kinematics.open_in_mokka now pops with focus, and added gui.set_color_order.
</commit_message>
<xml_diff>
--- a/conversion_state.xlsx
+++ b/conversion_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Documents/Recherche/pyKTK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2258DBFE-6D86-3F4E-9A65-D65E73194794}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C56364-C87C-7441-8E1A-73D5BB43C1DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="148">
   <si>
     <t>Module</t>
   </si>
@@ -463,6 +463,12 @@
   </si>
   <si>
     <t>Maybe transfer to "extract_cycles(start_event_name, stop_event_name)" that creates a dict of (n_cycles x 100 x data_dim) arrays</t>
+  </si>
+  <si>
+    <t>open_in_mokka</t>
+  </si>
+  <si>
+    <t>gui.set_color_order</t>
   </si>
 </sst>
 </file>
@@ -892,7 +898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF09E79-E66E-9E44-A75F-B1B1B21A0B2B}">
   <dimension ref="A1:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
@@ -1409,11 +1415,8 @@
       <c r="B42" t="s">
         <v>49</v>
       </c>
-      <c r="D42" t="s">
-        <v>90</v>
-      </c>
-      <c r="E42" t="s">
-        <v>92</v>
+      <c r="C42" t="s">
+        <v>147</v>
       </c>
       <c r="F42" t="s">
         <v>127</v>
@@ -1546,6 +1549,9 @@
       </c>
       <c r="B51" t="s">
         <v>60</v>
+      </c>
+      <c r="C51" t="s">
+        <v>146</v>
       </c>
       <c r="D51" t="s">
         <v>90</v>

</xml_diff>

<commit_message>
[STABLE] Added pushrimkinetics.calculate_velocity and calculate_power
</commit_message>
<xml_diff>
--- a/conversion_state.xlsx
+++ b/conversion_state.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Documents/Recherche/pyKTK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C56364-C87C-7441-8E1A-73D5BB43C1DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE578723-6765-9E43-A6AA-399A63749002}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="38360" windowHeight="21120" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="151">
   <si>
     <t>Module</t>
   </si>
@@ -204,9 +204,6 @@
     <t>exporttotrc</t>
   </si>
   <si>
-    <t>opentutorial</t>
-  </si>
-  <si>
     <t>playinmokka</t>
   </si>
   <si>
@@ -375,9 +372,6 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Should be included as an input flag to plot()</t>
-  </si>
-  <si>
     <t>Time is always first in Python</t>
   </si>
   <si>
@@ -469,6 +463,21 @@
   </si>
   <si>
     <t>gui.set_color_order</t>
+  </si>
+  <si>
+    <t>plot(plot_event_names=True)</t>
+  </si>
+  <si>
+    <t>Not necessary. One can simply print in the console or in message for long tasks.</t>
+  </si>
+  <si>
+    <t>Not sure if it's worth it. We can always print on console, and it looks like a hell of debugging.</t>
+  </si>
+  <si>
+    <t>calculate_power</t>
+  </si>
+  <si>
+    <t>calculate_velocity</t>
   </si>
 </sst>
 </file>
@@ -896,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF09E79-E66E-9E44-A75F-B1B1B21A0B2B}">
-  <dimension ref="A1:F95"/>
+  <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -920,16 +929,16 @@
         <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -940,7 +949,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -951,10 +960,10 @@
         <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -965,13 +974,13 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -982,7 +991,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -990,7 +999,7 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -998,7 +1007,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1006,10 +1015,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1017,7 +1026,7 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1025,7 +1034,7 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1036,7 +1045,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1044,7 +1053,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1052,7 +1061,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1063,7 +1072,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1071,7 +1080,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1103,14 +1112,8 @@
       <c r="B18" t="s">
         <v>17</v>
       </c>
-      <c r="D18" t="s">
-        <v>90</v>
-      </c>
-      <c r="E18" t="s">
-        <v>92</v>
-      </c>
-      <c r="F18" t="s">
-        <v>116</v>
+      <c r="C18" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1121,10 +1124,10 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1135,10 +1138,10 @@
         <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1149,10 +1152,10 @@
         <v>22</v>
       </c>
       <c r="D21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1163,13 +1166,13 @@
         <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F22" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1180,7 +1183,7 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1191,7 +1194,7 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1202,10 +1205,10 @@
         <v>26</v>
       </c>
       <c r="D25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E25" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1213,7 +1216,7 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1221,7 +1224,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1229,7 +1232,7 @@
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1240,10 +1243,10 @@
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1254,10 +1257,10 @@
         <v>29</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1268,7 +1271,7 @@
         <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1290,10 +1293,10 @@
         <v>33</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1304,10 +1307,10 @@
         <v>34</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E34" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1318,10 +1321,10 @@
         <v>35</v>
       </c>
       <c r="D35" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E35" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1332,10 +1335,10 @@
         <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E36" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1346,10 +1349,10 @@
         <v>37</v>
       </c>
       <c r="D37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E37" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1360,10 +1363,10 @@
         <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1374,10 +1377,10 @@
         <v>39</v>
       </c>
       <c r="D39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1388,10 +1391,10 @@
         <v>40</v>
       </c>
       <c r="D40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1402,10 +1405,10 @@
         <v>41</v>
       </c>
       <c r="D41" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E41" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1416,10 +1419,10 @@
         <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F42" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1430,30 +1433,27 @@
         <v>51</v>
       </c>
       <c r="D43" t="s">
-        <v>90</v>
+        <v>116</v>
       </c>
       <c r="E43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F43" t="s">
-        <v>127</v>
+        <v>148</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B44" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D44" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E44" t="s">
-        <v>114</v>
-      </c>
-      <c r="F44" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1461,13 +1461,13 @@
         <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E45" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1475,13 +1475,13 @@
         <v>53</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E46" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1489,13 +1489,16 @@
         <v>53</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D47" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E47" t="s">
-        <v>114</v>
+        <v>91</v>
+      </c>
+      <c r="F47" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1503,16 +1506,13 @@
         <v>53</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D48" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E48" t="s">
-        <v>92</v>
-      </c>
-      <c r="F48" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1520,13 +1520,19 @@
         <v>53</v>
       </c>
       <c r="B49" t="s">
-        <v>58</v>
+        <v>59</v>
+      </c>
+      <c r="C49" t="s">
+        <v>144</v>
       </c>
       <c r="D49" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E49" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="F49" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1534,13 +1540,13 @@
         <v>53</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D50" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1548,19 +1554,13 @@
         <v>53</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C51" t="s">
-        <v>146</v>
-      </c>
-      <c r="D51" t="s">
-        <v>90</v>
-      </c>
-      <c r="E51" t="s">
-        <v>92</v>
+        <v>138</v>
       </c>
       <c r="F51" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1568,13 +1568,13 @@
         <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D52" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E52" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1582,13 +1582,13 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
-      </c>
-      <c r="C53" t="s">
-        <v>140</v>
-      </c>
-      <c r="F53" t="s">
-        <v>139</v>
+        <v>64</v>
+      </c>
+      <c r="D53" t="s">
+        <v>89</v>
+      </c>
+      <c r="E53" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1596,326 +1596,323 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D54" t="s">
-        <v>118</v>
+        <v>89</v>
+      </c>
+      <c r="E54" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
-      </c>
-      <c r="D55" t="s">
-        <v>90</v>
-      </c>
-      <c r="E55" t="s">
-        <v>114</v>
+        <v>70</v>
+      </c>
+      <c r="C55" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
-      </c>
-      <c r="D56" t="s">
-        <v>90</v>
-      </c>
-      <c r="E56" t="s">
-        <v>92</v>
+        <v>71</v>
+      </c>
+      <c r="C56" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
-      </c>
-      <c r="D57" t="s">
-        <v>90</v>
-      </c>
-      <c r="E57" t="s">
-        <v>114</v>
+        <v>72</v>
+      </c>
+      <c r="C57" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B58" t="s">
-        <v>68</v>
-      </c>
-      <c r="D58" t="s">
-        <v>118</v>
-      </c>
-      <c r="F58" t="s">
+        <v>73</v>
+      </c>
+      <c r="C58" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B59" t="s">
-        <v>69</v>
-      </c>
-      <c r="D59" t="s">
-        <v>118</v>
-      </c>
-      <c r="F59" t="s">
-        <v>128</v>
+        <v>74</v>
+      </c>
+      <c r="C59" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B60" t="s">
-        <v>71</v>
-      </c>
-      <c r="C60" t="s">
-        <v>129</v>
+        <v>75</v>
+      </c>
+      <c r="D60" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B61" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D61" t="s">
-        <v>90</v>
-      </c>
-      <c r="E61" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B62" t="s">
-        <v>73</v>
-      </c>
-      <c r="D62" t="s">
-        <v>90</v>
-      </c>
-      <c r="E62" t="s">
-        <v>92</v>
+        <v>62</v>
+      </c>
+      <c r="C62" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B63" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C63" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B64" t="s">
-        <v>75</v>
-      </c>
-      <c r="C64" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+        <v>78</v>
+      </c>
+      <c r="D64" t="s">
+        <v>89</v>
+      </c>
+      <c r="E64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B65" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D65" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E65" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B66" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D66" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+        <v>89</v>
+      </c>
+      <c r="E66" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B67" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D67" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+        <v>89</v>
+      </c>
+      <c r="E67" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B68" t="s">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="C68" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:6">
       <c r="A69" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B69" t="s">
-        <v>78</v>
-      </c>
-      <c r="C69" t="s">
+        <v>84</v>
+      </c>
+      <c r="D69" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" t="s">
+        <v>80</v>
+      </c>
+      <c r="B70" t="s">
+        <v>85</v>
+      </c>
+      <c r="D70" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
-      <c r="A70" t="s">
-        <v>70</v>
-      </c>
-      <c r="B70" t="s">
-        <v>79</v>
-      </c>
-      <c r="D70" t="s">
-        <v>90</v>
-      </c>
-      <c r="E70" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
-      <c r="A71" t="s">
-        <v>80</v>
-      </c>
-      <c r="B71" t="s">
-        <v>63</v>
-      </c>
-      <c r="D71" t="s">
-        <v>90</v>
-      </c>
-      <c r="E71" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="C71" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" t="s">
-        <v>81</v>
-      </c>
-      <c r="B72" t="s">
-        <v>82</v>
-      </c>
-      <c r="D72" t="s">
-        <v>90</v>
-      </c>
-      <c r="E72" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
+        <v>133</v>
+      </c>
+      <c r="C72" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" t="s">
-        <v>81</v>
-      </c>
-      <c r="B73" t="s">
-        <v>83</v>
-      </c>
-      <c r="D73" t="s">
-        <v>90</v>
-      </c>
-      <c r="E73" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
+        <v>133</v>
+      </c>
+      <c r="C73" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B74" t="s">
-        <v>84</v>
-      </c>
-      <c r="C74" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
+        <v>67</v>
+      </c>
+      <c r="D74" t="s">
+        <v>116</v>
+      </c>
+      <c r="F74" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="B75" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="D75" t="s">
-        <v>90</v>
-      </c>
-      <c r="E75" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
+        <v>116</v>
+      </c>
+      <c r="F75" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" t="s">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
-      </c>
-      <c r="D76" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
+        <v>4</v>
+      </c>
+      <c r="C76" t="s">
+        <v>106</v>
+      </c>
+      <c r="F76" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77" t="s">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="B77" t="s">
-        <v>86</v>
-      </c>
-      <c r="D77" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
+        <v>5</v>
+      </c>
+      <c r="C77" t="s">
+        <v>106</v>
+      </c>
+      <c r="F77" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6">
       <c r="A78" t="s">
-        <v>135</v>
+        <v>1</v>
+      </c>
+      <c r="B78" t="s">
+        <v>6</v>
       </c>
       <c r="C78" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
+        <v>106</v>
+      </c>
+      <c r="F78" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" t="s">
-        <v>135</v>
+        <v>1</v>
+      </c>
+      <c r="B79" t="s">
+        <v>10</v>
       </c>
       <c r="C79" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
+        <v>106</v>
+      </c>
+      <c r="F79" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6">
       <c r="A80" t="s">
-        <v>135</v>
+        <v>1</v>
+      </c>
+      <c r="B80" t="s">
+        <v>11</v>
       </c>
       <c r="C80" t="s">
-        <v>138</v>
+        <v>106</v>
+      </c>
+      <c r="F80" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -1923,13 +1920,13 @@
         <v>1</v>
       </c>
       <c r="B81" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="C81" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F81" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -1937,13 +1934,13 @@
         <v>1</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C82" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F82" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -1951,83 +1948,83 @@
         <v>1</v>
       </c>
       <c r="B83" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C83" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F83" t="s">
-        <v>113</v>
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B84" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="C84" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F84" t="s">
-        <v>108</v>
+        <v>118</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B85" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="C85" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F85" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B86" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C86" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F86" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B87" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="C87" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F87" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B88" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="C88" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F88" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2035,13 +2032,13 @@
         <v>42</v>
       </c>
       <c r="B89" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C89" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F89" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2049,13 +2046,13 @@
         <v>42</v>
       </c>
       <c r="B90" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C90" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F90" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2063,78 +2060,33 @@
         <v>42</v>
       </c>
       <c r="B91" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C91" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F91" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B92" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C92" t="s">
-        <v>107</v>
-      </c>
-      <c r="F92" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
-      <c r="A93" t="s">
-        <v>42</v>
-      </c>
-      <c r="B93" t="s">
-        <v>47</v>
-      </c>
-      <c r="C93" t="s">
-        <v>107</v>
-      </c>
-      <c r="F93" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="A94" t="s">
-        <v>42</v>
-      </c>
-      <c r="B94" t="s">
-        <v>48</v>
-      </c>
-      <c r="C94" t="s">
-        <v>107</v>
-      </c>
-      <c r="F94" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" t="s">
-        <v>42</v>
-      </c>
-      <c r="B95" t="s">
-        <v>50</v>
-      </c>
-      <c r="C95" t="s">
-        <v>107</v>
-      </c>
-      <c r="F95" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A97:XFD97">
+  <conditionalFormatting sqref="A94:XFD94">
     <cfRule type="expression" dxfId="5" priority="8">
-      <formula>($C97&lt;&gt;"")</formula>
+      <formula>($C94&lt;&gt;"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:XFD96">
+  <conditionalFormatting sqref="A2:XFD93">
     <cfRule type="expression" dxfId="4" priority="4">
       <formula>($C2="N/A")</formula>
     </cfRule>
@@ -2142,17 +2094,17 @@
       <formula>AND(($C2&lt;&gt;""),($C2&lt;&gt;"N/A"))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:XFD96">
+  <conditionalFormatting sqref="A2:XFD93">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>($E2="easy")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:XFD96">
+  <conditionalFormatting sqref="A2:XFD93">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>($E2="moderate")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:XFD96">
+  <conditionalFormatting sqref="A2:XFD93">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>($E2="hard")</formula>
     </cfRule>

</xml_diff>

<commit_message>
Advances in ktk.cycles ; Started a tutorial for TimeSeries.
</commit_message>
<xml_diff>
--- a/conversion_state.xlsx
+++ b/conversion_state.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Documents/Recherche/pyKTK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37C0A5B-8A50-0E40-96D8-78F186F4B90D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639B0099-0B20-0C4C-920F-702B17F3B71C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="38360" windowHeight="21120" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
+    <workbookView xWindow="-28780" yWindow="2380" windowWidth="28760" windowHeight="17520" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="157">
   <si>
     <t>Module</t>
   </si>
@@ -438,9 +438,6 @@
     <t>get_folder</t>
   </si>
   <si>
-    <t>Using py-c3d which I just forked</t>
-  </si>
-  <si>
     <t>read_c3d_file</t>
   </si>
   <si>
@@ -453,9 +450,6 @@
     <t>ts.events = []</t>
   </si>
   <si>
-    <t>Maybe make a ktk.cycles submodule for cycle analysis</t>
-  </si>
-  <si>
     <t>Maybe transfer to "extract_cycles(start_event_name, stop_event_name)" that creates a dict of (n_cycles x 100 x data_dim) arrays</t>
   </si>
   <si>
@@ -493,6 +487,15 @@
   </si>
   <si>
     <t>ui_sync</t>
+  </si>
+  <si>
+    <t>Now using ezc3d to be up to date with different c3d formats</t>
+  </si>
+  <si>
+    <t>Will be in ktk.cycles</t>
+  </si>
+  <si>
+    <t>Not required, we can use sorted(ts.events) to get the events sorted.</t>
   </si>
 </sst>
 </file>
@@ -967,8 +970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF09E79-E66E-9E44-A75F-B1B1B21A0B2B}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1165,7 +1168,7 @@
         <v>106</v>
       </c>
       <c r="F14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1221,7 +1224,7 @@
         <v>106</v>
       </c>
       <c r="F18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1332,7 +1335,7 @@
         <v>91</v>
       </c>
       <c r="F27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1357,7 +1360,7 @@
         <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D29" t="s">
         <v>89</v>
@@ -1366,7 +1369,7 @@
         <v>91</v>
       </c>
       <c r="F29" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1391,10 +1394,10 @@
         <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F31" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1497,7 +1500,7 @@
         <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1508,7 +1511,7 @@
         <v>72</v>
       </c>
       <c r="C40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1630,7 +1633,7 @@
         <v>113</v>
       </c>
       <c r="F50" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1763,7 +1766,7 @@
         <v>17</v>
       </c>
       <c r="C64" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1773,11 +1776,8 @@
       <c r="B65" t="s">
         <v>18</v>
       </c>
-      <c r="D65" t="s">
-        <v>89</v>
-      </c>
-      <c r="E65" t="s">
-        <v>91</v>
+      <c r="C65" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1787,11 +1787,11 @@
       <c r="B66" t="s">
         <v>21</v>
       </c>
-      <c r="D66" t="s">
-        <v>89</v>
-      </c>
-      <c r="E66" t="s">
-        <v>91</v>
+      <c r="C66" t="s">
+        <v>106</v>
+      </c>
+      <c r="F66" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1822,7 +1822,7 @@
         <v>113</v>
       </c>
       <c r="F68" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1855,7 +1855,7 @@
         <v>26</v>
       </c>
       <c r="C71" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1991,7 +1991,7 @@
         <v>106</v>
       </c>
       <c r="F82" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -1999,7 +1999,7 @@
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2007,7 +2007,7 @@
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2018,7 +2018,7 @@
         <v>49</v>
       </c>
       <c r="C85" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F85" t="s">
         <v>125</v>
@@ -2032,7 +2032,7 @@
         <v>51</v>
       </c>
       <c r="C86" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2144,7 +2144,7 @@
         <v>106</v>
       </c>
       <c r="F94" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added and tested create_reference_frame. get_local_coordinates doesn't work as expected for now.
</commit_message>
<xml_diff>
--- a/conversion_state.xlsx
+++ b/conversion_state.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Documents/Recherche/pyKTK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{639B0099-0B20-0C4C-920F-702B17F3B71C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55ABBAB-2141-1245-ACA8-E3C80431509A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28780" yWindow="2380" windowWidth="28760" windowHeight="17520" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="38360" windowHeight="21120" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="158">
   <si>
     <t>Module</t>
   </si>
@@ -496,6 +496,9 @@
   </si>
   <si>
     <t>Not required, we can use sorted(ts.events) to get the events sorted.</t>
+  </si>
+  <si>
+    <t>No need, implemented directly into create_reference_frame. Could move it out if needed.</t>
   </si>
 </sst>
 </file>
@@ -970,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF09E79-E66E-9E44-A75F-B1B1B21A0B2B}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="F68" sqref="F68"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1234,11 +1237,11 @@
       <c r="B19" t="s">
         <v>40</v>
       </c>
-      <c r="D19" t="s">
-        <v>89</v>
-      </c>
-      <c r="E19" t="s">
-        <v>91</v>
+      <c r="C19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F19" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:6">

</xml_diff>

<commit_message>
[STABLE] ktk.geometry.create_reference_frame, ktk.geometry.get_local_coordinates, ktk.geometry.get_global_coordinates. All tested and documented.
</commit_message>
<xml_diff>
--- a/conversion_state.xlsx
+++ b/conversion_state.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Documents/Recherche/pyKTK/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55ABBAB-2141-1245-ACA8-E3C80431509A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF423EA-E717-DC4D-A561-B74998AD9892}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="38360" windowHeight="21120" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28760" windowHeight="17520" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="161">
   <si>
     <t>Module</t>
   </si>
@@ -450,9 +450,6 @@
     <t>ts.events = []</t>
   </si>
   <si>
-    <t>Maybe transfer to "extract_cycles(start_event_name, stop_event_name)" that creates a dict of (n_cycles x 100 x data_dim) arrays</t>
-  </si>
-  <si>
     <t>open_in_mokka</t>
   </si>
   <si>
@@ -499,6 +496,18 @@
   </si>
   <si>
     <t>No need, implemented directly into create_reference_frame. Could move it out if needed.</t>
+  </si>
+  <si>
+    <t>create_reference_frame</t>
+  </si>
+  <si>
+    <t>get_global_coordinates</t>
+  </si>
+  <si>
+    <t>get_local_coordinates</t>
+  </si>
+  <si>
+    <t>ktk.cycles.time_normalize</t>
   </si>
 </sst>
 </file>
@@ -973,8 +982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF09E79-E66E-9E44-A75F-B1B1B21A0B2B}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1139,11 +1148,8 @@
       <c r="B12" t="s">
         <v>33</v>
       </c>
-      <c r="D12" t="s">
-        <v>89</v>
-      </c>
-      <c r="E12" t="s">
-        <v>91</v>
+      <c r="C12" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1171,7 +1177,7 @@
         <v>106</v>
       </c>
       <c r="F14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1195,11 +1201,8 @@
       <c r="B16" t="s">
         <v>37</v>
       </c>
-      <c r="D16" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" t="s">
-        <v>113</v>
+      <c r="C16" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1209,11 +1212,8 @@
       <c r="B17" t="s">
         <v>38</v>
       </c>
-      <c r="D17" t="s">
-        <v>89</v>
-      </c>
-      <c r="E17" t="s">
-        <v>113</v>
+      <c r="C17" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1227,7 +1227,7 @@
         <v>106</v>
       </c>
       <c r="F18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1241,7 +1241,7 @@
         <v>106</v>
       </c>
       <c r="F19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1363,7 +1363,7 @@
         <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D29" t="s">
         <v>89</v>
@@ -1400,7 +1400,7 @@
         <v>137</v>
       </c>
       <c r="F31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1503,7 +1503,7 @@
         <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1514,7 +1514,7 @@
         <v>72</v>
       </c>
       <c r="C40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1636,7 +1636,7 @@
         <v>113</v>
       </c>
       <c r="F50" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1769,7 +1769,7 @@
         <v>17</v>
       </c>
       <c r="C64" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1794,7 +1794,7 @@
         <v>106</v>
       </c>
       <c r="F66" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1818,14 +1818,8 @@
       <c r="B68" t="s">
         <v>23</v>
       </c>
-      <c r="D68" t="s">
-        <v>89</v>
-      </c>
-      <c r="E68" t="s">
-        <v>113</v>
-      </c>
-      <c r="F68" t="s">
-        <v>141</v>
+      <c r="C68" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1858,7 +1852,7 @@
         <v>26</v>
       </c>
       <c r="C71" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -2002,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2010,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2021,7 +2015,7 @@
         <v>49</v>
       </c>
       <c r="C85" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F85" t="s">
         <v>125</v>
@@ -2035,7 +2029,7 @@
         <v>51</v>
       </c>
       <c r="C86" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2147,7 +2141,7 @@
         <v>106</v>
       </c>
       <c r="F94" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added functions to register points/markers in geometry/kinematics.
</commit_message>
<xml_diff>
--- a/conversion_state.xlsx
+++ b/conversion_state.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Documents/Recherche/pyKTK/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Documents/Recherche/kineticstoolkit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A259573-B97D-4645-AC6B-4ED33054C73E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8164D032-5EDE-124C-9028-D514F8CE3151}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4080" windowWidth="28760" windowHeight="17520" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="28760" windowHeight="17520" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="165">
   <si>
     <t>Module</t>
   </si>
@@ -517,6 +517,9 @@
   </si>
   <si>
     <t>create_rotation_matrix</t>
+  </si>
+  <si>
+    <t>create_rigid_body_config</t>
   </si>
 </sst>
 </file>
@@ -992,7 +995,7 @@
   <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1295,11 +1298,8 @@
       <c r="B24" t="s">
         <v>54</v>
       </c>
-      <c r="D24" t="s">
-        <v>89</v>
-      </c>
-      <c r="E24" t="s">
-        <v>113</v>
+      <c r="C24" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:6">

</xml_diff>

<commit_message>
[STABLE] We now have a complete workflow from reading c3d/n3d to recreating all virtual markers using probing acquisitions.
</commit_message>
<xml_diff>
--- a/conversion_state.xlsx
+++ b/conversion_state.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Documents/Recherche/kineticstoolkit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8164D032-5EDE-124C-9028-D514F8CE3151}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D11C71-806B-7C4D-90B0-5C9C7A5FC328}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="28760" windowHeight="17520" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="170">
   <si>
     <t>Module</t>
   </si>
@@ -520,6 +520,21 @@
   </si>
   <si>
     <t>create_rigid_body_config</t>
+  </si>
+  <si>
+    <t>register_points</t>
+  </si>
+  <si>
+    <t>read_n3d_file</t>
+  </si>
+  <si>
+    <t>register_markers</t>
+  </si>
+  <si>
+    <t>create_virtual_marker_config</t>
+  </si>
+  <si>
+    <t>No need to, since we can calculate rigid bodies using real and virtual markers following ISB</t>
   </si>
 </sst>
 </file>
@@ -994,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF09E79-E66E-9E44-A75F-B1B1B21A0B2B}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1260,11 +1275,8 @@
       <c r="B20" t="s">
         <v>41</v>
       </c>
-      <c r="D20" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" t="s">
-        <v>113</v>
+      <c r="C20" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1309,11 +1321,8 @@
       <c r="B25" t="s">
         <v>55</v>
       </c>
-      <c r="D25" t="s">
-        <v>89</v>
-      </c>
-      <c r="E25" t="s">
-        <v>113</v>
+      <c r="C25" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1323,11 +1332,11 @@
       <c r="B26" t="s">
         <v>56</v>
       </c>
-      <c r="D26" t="s">
-        <v>89</v>
-      </c>
-      <c r="E26" t="s">
-        <v>113</v>
+      <c r="C26" t="s">
+        <v>106</v>
+      </c>
+      <c r="F26" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1416,11 +1425,8 @@
       <c r="B32" t="s">
         <v>63</v>
       </c>
-      <c r="D32" t="s">
-        <v>89</v>
-      </c>
-      <c r="E32" t="s">
-        <v>113</v>
+      <c r="C32" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1444,11 +1450,8 @@
       <c r="B34" t="s">
         <v>65</v>
       </c>
-      <c r="D34" t="s">
-        <v>89</v>
-      </c>
-      <c r="E34" t="s">
-        <v>113</v>
+      <c r="C34" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="1:6">

</xml_diff>

<commit_message>
Unit tests are now launched in a separate process to avoid zombie matplotlib windows after running tests.
</commit_message>
<xml_diff>
--- a/conversion_state.xlsx
+++ b/conversion_state.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felix/Documents/Recherche/kineticstoolkit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D11C71-806B-7C4D-90B0-5C9C7A5FC328}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B446DF1-26B2-5D46-9C57-E504612FBFB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="480" windowWidth="28760" windowHeight="17520" xr2:uid="{14DC2B4B-2BFB-1245-B107-F21DDCB2CAE0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="172">
   <si>
     <t>Module</t>
   </si>
@@ -438,18 +438,9 @@
     <t>read_c3d_file</t>
   </si>
   <si>
-    <t>to become write_mvc_file (for the segments)</t>
-  </si>
-  <si>
-    <t>I modified py-c3d. Not yet working on Windows, just have to launch the command line correctly.</t>
-  </si>
-  <si>
     <t>ts.events = []</t>
   </si>
   <si>
-    <t>open_in_mokka</t>
-  </si>
-  <si>
     <t>gui.set_color_order</t>
   </si>
   <si>
@@ -507,12 +498,6 @@
     <t>ktk.cycles.time_normalize</t>
   </si>
   <si>
-    <t>Will implement a close callback on the figure instead, if needed.</t>
-  </si>
-  <si>
-    <t>hard</t>
-  </si>
-  <si>
     <t>Design choices to do</t>
   </si>
   <si>
@@ -535,13 +520,34 @@
   </si>
   <si>
     <t>No need to, since we can calculate rigid bodies using real and virtual markers following ISB</t>
+  </si>
+  <si>
+    <t>Player is capable now.</t>
+  </si>
+  <si>
+    <t>fill_missing_samples</t>
+  </si>
+  <si>
+    <t>create_file_entry</t>
+  </si>
+  <si>
+    <t>Integrated in the File table</t>
+  </si>
+  <si>
+    <t>Integrated in DBInterface.save</t>
+  </si>
+  <si>
+    <t>We must choose our filter to differenciate.</t>
+  </si>
+  <si>
+    <t>sync_on_event</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1009,11 +1015,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF09E79-E66E-9E44-A75F-B1B1B21A0B2B}">
   <dimension ref="A1:F94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" bestFit="1" customWidth="1"/>
@@ -1023,7 +1029,7 @@
     <col min="6" max="6" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1043,35 +1049,32 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>80</v>
       </c>
       <c r="B2" t="s">
         <v>81</v>
       </c>
-      <c r="D2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="C2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>80</v>
       </c>
       <c r="B3" t="s">
         <v>82</v>
       </c>
-      <c r="D3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>80</v>
       </c>
@@ -1082,29 +1085,35 @@
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>80</v>
       </c>
       <c r="B5" t="s">
         <v>84</v>
       </c>
-      <c r="D5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="C5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>80</v>
       </c>
       <c r="B6" t="s">
         <v>85</v>
       </c>
-      <c r="D6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="C6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -1118,35 +1127,32 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>27</v>
       </c>
       <c r="B8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
-        <v>89</v>
-      </c>
-      <c r="E8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
       </c>
-      <c r="D9" t="s">
-        <v>89</v>
-      </c>
-      <c r="E9" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="C9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1157,7 +1163,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1168,7 +1174,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1176,10 +1182,10 @@
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1187,10 +1193,10 @@
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -1201,10 +1207,10 @@
         <v>106</v>
       </c>
       <c r="F14" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1218,7 +1224,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1226,10 +1232,10 @@
         <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1237,10 +1243,10 @@
         <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1251,10 +1257,10 @@
         <v>106</v>
       </c>
       <c r="F18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>32</v>
       </c>
@@ -1265,10 +1271,10 @@
         <v>106</v>
       </c>
       <c r="F19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>32</v>
       </c>
@@ -1276,10 +1282,10 @@
         <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>132</v>
       </c>
@@ -1287,7 +1293,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>132</v>
       </c>
@@ -1295,7 +1301,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>132</v>
       </c>
@@ -1303,7 +1309,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>53</v>
       </c>
@@ -1311,10 +1317,10 @@
         <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1322,10 +1328,10 @@
         <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -1336,27 +1342,24 @@
         <v>106</v>
       </c>
       <c r="F26" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>53</v>
       </c>
       <c r="B27" t="s">
         <v>57</v>
       </c>
-      <c r="D27" t="s">
-        <v>89</v>
-      </c>
-      <c r="E27" t="s">
-        <v>91</v>
+      <c r="C27" t="s">
+        <v>106</v>
       </c>
       <c r="F27" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -1370,7 +1373,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -1378,19 +1381,13 @@
         <v>59</v>
       </c>
       <c r="C29" t="s">
-        <v>140</v>
-      </c>
-      <c r="D29" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="F29" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1404,7 +1401,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -1415,10 +1412,10 @@
         <v>136</v>
       </c>
       <c r="F31" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>53</v>
       </c>
@@ -1426,10 +1423,10 @@
         <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -1443,7 +1440,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -1451,10 +1448,10 @@
         <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>53</v>
       </c>
@@ -1465,7 +1462,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>66</v>
       </c>
@@ -1473,13 +1470,10 @@
         <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
-      </c>
-      <c r="F36" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>66</v>
       </c>
@@ -1490,13 +1484,13 @@
         <v>89</v>
       </c>
       <c r="E37" t="s">
-        <v>161</v>
+        <v>113</v>
       </c>
       <c r="F37" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>69</v>
       </c>
@@ -1507,7 +1501,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>69</v>
       </c>
@@ -1515,10 +1509,10 @@
         <v>71</v>
       </c>
       <c r="C39" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -1526,10 +1520,10 @@
         <v>72</v>
       </c>
       <c r="C40" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>69</v>
       </c>
@@ -1540,7 +1534,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>69</v>
       </c>
@@ -1551,7 +1545,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>69</v>
       </c>
@@ -1562,7 +1556,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>69</v>
       </c>
@@ -1573,7 +1567,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>69</v>
       </c>
@@ -1584,7 +1578,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>69</v>
       </c>
@@ -1595,7 +1589,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>69</v>
       </c>
@@ -1609,7 +1603,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>1</v>
       </c>
@@ -1620,21 +1614,18 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>1</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
       </c>
-      <c r="D49" t="s">
-        <v>89</v>
-      </c>
-      <c r="E49" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+      <c r="C49" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>1</v>
       </c>
@@ -1648,10 +1639,10 @@
         <v>113</v>
       </c>
       <c r="F50" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>1</v>
       </c>
@@ -1662,7 +1653,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>1</v>
       </c>
@@ -1670,7 +1661,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>1</v>
       </c>
@@ -1678,7 +1669,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>1</v>
       </c>
@@ -1689,7 +1680,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>1</v>
       </c>
@@ -1697,7 +1688,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -1705,7 +1696,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>1</v>
       </c>
@@ -1716,7 +1707,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>1</v>
       </c>
@@ -1724,7 +1715,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>1</v>
       </c>
@@ -1732,7 +1723,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>1</v>
       </c>
@@ -1743,7 +1734,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>1</v>
       </c>
@@ -1751,7 +1742,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>1</v>
       </c>
@@ -1762,7 +1753,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>1</v>
       </c>
@@ -1773,7 +1764,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>1</v>
       </c>
@@ -1781,10 +1772,10 @@
         <v>17</v>
       </c>
       <c r="C64" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>1</v>
       </c>
@@ -1795,7 +1786,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>1</v>
       </c>
@@ -1806,24 +1797,21 @@
         <v>106</v>
       </c>
       <c r="F66" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>1</v>
       </c>
       <c r="B67" t="s">
         <v>22</v>
       </c>
-      <c r="D67" t="s">
-        <v>89</v>
-      </c>
-      <c r="E67" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+      <c r="C67" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>1</v>
       </c>
@@ -1831,10 +1819,10 @@
         <v>23</v>
       </c>
       <c r="C68" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>1</v>
       </c>
@@ -1845,7 +1833,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>1</v>
       </c>
@@ -1856,7 +1844,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>1</v>
       </c>
@@ -1864,10 +1852,10 @@
         <v>26</v>
       </c>
       <c r="C71" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>1</v>
       </c>
@@ -1875,7 +1863,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>1</v>
       </c>
@@ -1883,7 +1871,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>1</v>
       </c>
@@ -1891,7 +1879,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>1</v>
       </c>
@@ -1905,7 +1893,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>1</v>
       </c>
@@ -1919,7 +1907,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>1</v>
       </c>
@@ -1933,7 +1921,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>1</v>
       </c>
@@ -1947,7 +1935,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -1961,7 +1949,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>1</v>
       </c>
@@ -1975,7 +1963,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>1</v>
       </c>
@@ -1989,7 +1977,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>1</v>
       </c>
@@ -2000,26 +1988,26 @@
         <v>106</v>
       </c>
       <c r="F82" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>1</v>
       </c>
       <c r="C83" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>1</v>
       </c>
       <c r="C84" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>42</v>
       </c>
@@ -2027,13 +2015,13 @@
         <v>49</v>
       </c>
       <c r="C85" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="F85" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>42</v>
       </c>
@@ -2041,10 +2029,10 @@
         <v>51</v>
       </c>
       <c r="C86" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>42</v>
       </c>
@@ -2058,7 +2046,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>42</v>
       </c>
@@ -2072,7 +2060,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>42</v>
       </c>
@@ -2086,7 +2074,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>42</v>
       </c>
@@ -2100,7 +2088,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>42</v>
       </c>
@@ -2114,7 +2102,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>42</v>
       </c>
@@ -2128,7 +2116,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>42</v>
       </c>
@@ -2142,7 +2130,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>42</v>
       </c>
@@ -2153,11 +2141,11 @@
         <v>106</v>
       </c>
       <c r="F94" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:F94">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F94">
     <sortCondition ref="A2:A94"/>
   </sortState>
   <conditionalFormatting sqref="B94:XFD94">
@@ -2188,27 +2176,27 @@
       <formula>($E2="hard")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
+  <conditionalFormatting sqref="A90:XFD96">
     <cfRule type="expression" dxfId="4" priority="4">
-      <formula>($C94="N/A")</formula>
+      <formula>($C90="N/A")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="5">
-      <formula>AND(($C94&lt;&gt;""),($C94&lt;&gt;"N/A"))</formula>
+      <formula>AND(($C90&lt;&gt;""),($C90&lt;&gt;"N/A"))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
+  <conditionalFormatting sqref="A90:XFD96">
     <cfRule type="expression" dxfId="2" priority="3">
-      <formula>($E94="easy")</formula>
+      <formula>($E90="easy")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
+  <conditionalFormatting sqref="A90:XFD96">
     <cfRule type="expression" dxfId="1" priority="2">
-      <formula>($E94="moderate")</formula>
+      <formula>($E90="moderate")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A94">
+  <conditionalFormatting sqref="A90:XFD96">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>($E94="hard")</formula>
+      <formula>($E90="hard")</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>